<commit_message>
added last 100 averaging
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawesl\Documents\Computing\comp9444\hw3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldawe\Documents\computing\comp9444\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23436" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23430" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>cartpole</t>
   </si>
@@ -73,13 +74,27 @@
   <si>
     <t>too unstable</t>
   </si>
+  <si>
+    <t>L2 beta</t>
+  </si>
+  <si>
+    <t>best av 100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,9 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,7 +147,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -142,7 +161,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -282,6 +300,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5542-4189-A633-F92C8BE68F3A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -343,7 +366,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$15</c:f>
+              <c:f>Sheet1!$L$4:$L$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -380,6 +403,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5542-4189-A633-F92C8BE68F3A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -441,7 +469,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$15</c:f>
+              <c:f>Sheet1!$M$4:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -478,6 +506,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5542-4189-A633-F92C8BE68F3A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -609,7 +642,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1223,20 +1255,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>144780</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1550,34 +1588,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="13" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1608,8 +1647,11 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1640,14 +1682,14 @@
       <c r="J4">
         <v>13</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>11.42</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>11.06</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1678,14 +1720,14 @@
       <c r="J5">
         <v>11.52</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>34.74</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1716,14 +1758,14 @@
       <c r="J6">
         <v>26.56</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>13.28</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1754,14 +1796,14 @@
       <c r="J7">
         <v>15.77</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>105.12</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>89.45</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1792,14 +1834,14 @@
       <c r="J8">
         <v>79.45</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>95.62</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>90.19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1830,14 +1872,14 @@
       <c r="J9">
         <v>51.5</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>105.91</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>94.49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1868,15 +1910,15 @@
       <c r="J10">
         <v>98.81</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <f>(108.14 + 105.07) / 2</f>
         <v>106.60499999999999</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>85.15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1908,15 +1950,15 @@
         <f>(126.58 + 105.15)/2</f>
         <v>115.86500000000001</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <f>(108.4 + 97.6) / 2</f>
         <v>103</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>100.5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1947,15 +1989,15 @@
       <c r="J12">
         <v>97.39</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <f>(103.91 + 83.17) / 2</f>
         <v>93.539999999999992</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>87.58</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1986,15 +2028,15 @@
       <c r="J13">
         <v>119.87</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <f xml:space="preserve"> (95.16 + 66.89) / 2</f>
         <v>81.025000000000006</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>83.45</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2026,7 +2068,7 @@
         <v>107.38</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2058,7 +2100,7 @@
         <v>115.39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2090,7 +2132,7 @@
         <v>11.42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2122,7 +2164,7 @@
         <v>34.74</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2154,7 +2196,7 @@
         <v>13.28</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2186,7 +2228,7 @@
         <v>105.12</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2218,7 +2260,7 @@
         <v>95.62</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2250,7 +2292,7 @@
         <v>105.91</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2283,7 +2325,7 @@
         <v>106.60499999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2316,7 +2358,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2349,7 +2391,7 @@
         <v>93.539999999999992</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2382,7 +2424,7 @@
         <v>81.025000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2414,7 +2456,7 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2446,7 +2488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2478,7 +2520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2510,7 +2552,7 @@
         <v>89.45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2542,7 +2584,7 @@
         <v>90.19</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2574,7 +2616,7 @@
         <v>94.49</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2606,7 +2648,7 @@
         <v>85.15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2638,7 +2680,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2670,7 +2712,7 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2702,18 +2744,18 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="J39" t="s">
         <v>12</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2744,15 +2786,15 @@
       <c r="J40">
         <v>1000</v>
       </c>
-      <c r="K40" s="1">
+      <c r="L40" s="1">
         <v>105.74</v>
       </c>
-      <c r="L40" s="1">
+      <c r="M40" s="1">
         <f>(132.56 + 127.728) / 2</f>
         <v>130.14400000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2783,11 +2825,11 @@
       <c r="J41">
         <v>512</v>
       </c>
-      <c r="K41" s="1">
+      <c r="L41" s="1">
         <v>119.32299999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2818,11 +2860,11 @@
       <c r="J42">
         <v>2</v>
       </c>
-      <c r="K42" s="1">
+      <c r="L42" s="1">
         <v>139.5</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -2853,11 +2895,11 @@
       <c r="J43">
         <v>4</v>
       </c>
-      <c r="K43" s="1">
+      <c r="L43" s="1">
         <v>140.601</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -2888,11 +2930,11 @@
       <c r="J44">
         <v>64</v>
       </c>
-      <c r="K44" s="1">
+      <c r="L44" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2923,11 +2965,11 @@
       <c r="J45">
         <v>16</v>
       </c>
-      <c r="K45" s="1">
+      <c r="L45" s="1">
         <v>131.86500000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2958,11 +3000,11 @@
       <c r="J46">
         <v>8</v>
       </c>
-      <c r="K46" s="1">
+      <c r="L46" s="1">
         <v>135.36799999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2993,11 +3035,14 @@
       <c r="J47">
         <v>6</v>
       </c>
-      <c r="K47" s="1">
+      <c r="L47" s="1">
         <v>135.114</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -3028,11 +3073,14 @@
       <c r="J48">
         <v>4</v>
       </c>
-      <c r="K48" s="1">
+      <c r="L48" s="1">
         <v>164.054</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" s="1">
+        <v>193.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -3063,125 +3111,299 @@
       <c r="J49">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="K49">
+        <v>0.1</v>
+      </c>
+      <c r="L49" s="1">
+        <v>140.619</v>
+      </c>
+      <c r="M49" s="1">
+        <v>168.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>2</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>100</v>
+      </c>
+      <c r="F50" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G50" s="2">
+        <v>256</v>
+      </c>
+      <c r="H50" s="2">
+        <v>128</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J50" s="2">
+        <v>4</v>
+      </c>
+      <c r="K50" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="L50" s="3">
+        <v>177.71600000000001</v>
+      </c>
+      <c r="M50" s="3">
+        <v>196.95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>2</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="4">
+        <v>100</v>
+      </c>
+      <c r="F51" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G51" s="4">
+        <v>256</v>
+      </c>
+      <c r="H51" s="4">
+        <v>128</v>
+      </c>
+      <c r="I51" s="4">
+        <v>1000</v>
+      </c>
+      <c r="J51" s="4">
+        <v>4</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="L51" s="5">
+        <v>171.38900000000001</v>
+      </c>
+      <c r="M51" s="5">
+        <v>189.68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>2</v>
       </c>
-      <c r="B52">
-        <v>0.9</v>
-      </c>
-      <c r="C52">
-        <v>0.6</v>
-      </c>
-      <c r="D52">
-        <v>0.1</v>
-      </c>
-      <c r="E52">
-        <v>100</v>
-      </c>
-      <c r="F52">
-        <v>10000</v>
-      </c>
-      <c r="G52">
-        <v>128</v>
-      </c>
-      <c r="H52">
-        <v>128</v>
-      </c>
-      <c r="I52">
+      <c r="B54">
+        <v>0.9</v>
+      </c>
+      <c r="C54">
+        <v>0.6</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54">
+        <v>10000</v>
+      </c>
+      <c r="G54">
+        <v>128</v>
+      </c>
+      <c r="H54">
+        <v>128</v>
+      </c>
+      <c r="I54">
         <v>1000</v>
       </c>
-      <c r="J52">
+      <c r="J54">
         <v>4</v>
       </c>
-      <c r="K52" s="1">
+      <c r="L54" s="1">
         <f>(-195.396-197.553) / 2</f>
         <v>-196.47449999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>2</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>0.99</v>
       </c>
-      <c r="C53">
-        <v>0.6</v>
-      </c>
-      <c r="D53">
-        <v>0.1</v>
-      </c>
-      <c r="E53">
-        <v>100</v>
-      </c>
-      <c r="F53">
-        <v>10000</v>
-      </c>
-      <c r="G53">
-        <v>128</v>
-      </c>
-      <c r="H53">
-        <v>128</v>
-      </c>
-      <c r="I53">
+      <c r="C55">
+        <v>0.6</v>
+      </c>
+      <c r="D55">
+        <v>0.1</v>
+      </c>
+      <c r="E55">
+        <v>100</v>
+      </c>
+      <c r="F55">
+        <v>10000</v>
+      </c>
+      <c r="G55">
+        <v>128</v>
+      </c>
+      <c r="H55">
+        <v>128</v>
+      </c>
+      <c r="I55">
         <v>1000</v>
       </c>
-      <c r="J53">
+      <c r="J55">
         <v>4</v>
       </c>
-      <c r="K53" s="1">
+      <c r="L55" s="1">
         <v>-141.59899999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>2</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>0.999</v>
       </c>
-      <c r="C54">
-        <v>0.6</v>
-      </c>
-      <c r="D54">
-        <v>0.1</v>
-      </c>
-      <c r="E54">
-        <v>100</v>
-      </c>
-      <c r="F54">
-        <v>10000</v>
-      </c>
-      <c r="G54">
-        <v>128</v>
-      </c>
-      <c r="H54">
-        <v>128</v>
-      </c>
-      <c r="I54">
+      <c r="C56">
+        <v>0.6</v>
+      </c>
+      <c r="D56">
+        <v>0.1</v>
+      </c>
+      <c r="E56">
+        <v>100</v>
+      </c>
+      <c r="F56">
+        <v>10000</v>
+      </c>
+      <c r="G56">
+        <v>128</v>
+      </c>
+      <c r="H56">
+        <v>128</v>
+      </c>
+      <c r="I56">
         <v>1000</v>
       </c>
-      <c r="J54">
+      <c r="J56">
         <v>4</v>
       </c>
-      <c r="K54" s="1">
+      <c r="L56" s="1">
         <v>-140.88</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L55" s="1" t="s">
+      <c r="M56" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57">
+        <v>0.99</v>
+      </c>
+      <c r="C57">
+        <v>0.6</v>
+      </c>
+      <c r="D57">
+        <v>0.1</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57">
+        <v>10000</v>
+      </c>
+      <c r="G57">
+        <v>128</v>
+      </c>
+      <c r="H57">
+        <v>128</v>
+      </c>
+      <c r="I57">
+        <v>1000</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="K57">
+        <v>0.01</v>
+      </c>
+      <c r="L57" s="1">
+        <v>-199.65</v>
+      </c>
+      <c r="M57" s="1">
+        <v>-198.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>0.99</v>
+      </c>
+      <c r="C58">
+        <v>0.6</v>
+      </c>
+      <c r="D58">
+        <v>0.1</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58">
+        <v>10000</v>
+      </c>
+      <c r="G58">
+        <v>128</v>
+      </c>
+      <c r="H58">
+        <v>128</v>
+      </c>
+      <c r="I58">
+        <v>1000</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <v>1E-3</v>
+      </c>
+      <c r="L58" s="1">
+        <f>(-175.243-162.111) / 2</f>
+        <v>-168.67699999999999</v>
+      </c>
+      <c r="M58" s="1">
+        <f>(-125.35-114.61) / 2</f>
+        <v>-119.97999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
neural_qtrain ready for submission
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldawe\Documents\computing\comp9444\hw3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawesl\Documents\Computing\comp9444\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23430" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23436" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>cartpole</t>
   </si>
@@ -80,11 +79,35 @@
   <si>
     <t>best av 100</t>
   </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>top_100_av</t>
+  </si>
+  <si>
+    <t>var gamma</t>
+  </si>
+  <si>
+    <t>0.95-0.99</t>
+  </si>
+  <si>
+    <t>?fluke</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +170,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -161,6 +184,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -300,7 +324,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5542-4189-A633-F92C8BE68F3A}"/>
             </c:ext>
@@ -403,7 +427,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5542-4189-A633-F92C8BE68F3A}"/>
             </c:ext>
@@ -506,7 +530,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5542-4189-A633-F92C8BE68F3A}"/>
             </c:ext>
@@ -522,11 +546,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="385810104"/>
-        <c:axId val="385810496"/>
+        <c:axId val="354033280"/>
+        <c:axId val="354033672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="385810104"/>
+        <c:axId val="354033280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385810496"/>
+        <c:crossAx val="354033672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -577,7 +601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="385810496"/>
+        <c:axId val="354033672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385810104"/>
+        <c:crossAx val="354033280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,6 +666,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1271,7 +1296,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1588,35 +1613,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" customWidth="1"/>
+    <col min="12" max="13" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1651,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1689,7 +1714,7 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1727,7 +1752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1765,7 +1790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1803,7 +1828,7 @@
         <v>89.45</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1841,7 +1866,7 @@
         <v>90.19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1879,7 +1904,7 @@
         <v>94.49</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1918,7 +1943,7 @@
         <v>85.15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1958,7 +1983,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1997,7 +2022,7 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2036,7 +2061,7 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2068,7 +2093,7 @@
         <v>107.38</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2100,7 +2125,7 @@
         <v>115.39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2132,7 +2157,7 @@
         <v>11.42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2164,7 +2189,7 @@
         <v>34.74</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2196,7 +2221,7 @@
         <v>13.28</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2228,7 +2253,7 @@
         <v>105.12</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2260,7 +2285,7 @@
         <v>95.62</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2292,7 +2317,7 @@
         <v>105.91</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2325,7 +2350,7 @@
         <v>106.60499999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2358,7 +2383,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2391,7 +2416,7 @@
         <v>93.539999999999992</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2424,7 +2449,7 @@
         <v>81.025000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2456,7 +2481,7 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2488,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2520,7 +2545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2552,7 +2577,7 @@
         <v>89.45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2584,7 +2609,7 @@
         <v>90.19</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2616,7 +2641,7 @@
         <v>94.49</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2648,7 +2673,7 @@
         <v>85.15</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2680,7 +2705,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2712,7 +2737,7 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2744,7 +2769,7 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2794,7 +2819,7 @@
         <v>130.14400000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2829,7 +2854,7 @@
         <v>119.32299999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2864,7 +2889,7 @@
         <v>139.5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -2899,7 +2924,7 @@
         <v>140.601</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -2934,7 +2959,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2969,7 +2994,7 @@
         <v>131.86500000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -3004,7 +3029,7 @@
         <v>135.36799999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -3042,7 +3067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -3080,7 +3105,7 @@
         <v>193.1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -3121,7 +3146,7 @@
         <v>168.1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -3162,7 +3187,7 @@
         <v>196.95</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>2</v>
       </c>
@@ -3203,12 +3228,12 @@
         <v>189.68</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3228,7 +3253,7 @@
         <v>10000</v>
       </c>
       <c r="G54">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="H54">
         <v>128</v>
@@ -3244,7 +3269,7 @@
         <v>-196.47449999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3264,7 +3289,7 @@
         <v>10000</v>
       </c>
       <c r="G55">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="H55">
         <v>128</v>
@@ -3279,7 +3304,7 @@
         <v>-141.59899999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3299,7 +3324,7 @@
         <v>10000</v>
       </c>
       <c r="G56">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="H56">
         <v>128</v>
@@ -3317,7 +3342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3337,7 +3362,7 @@
         <v>10000</v>
       </c>
       <c r="G57">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="H57">
         <v>128</v>
@@ -3358,7 +3383,7 @@
         <v>-198.1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
@@ -3378,7 +3403,7 @@
         <v>10000</v>
       </c>
       <c r="G58">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="H58">
         <v>128</v>
@@ -3399,6 +3424,123 @@
       <c r="M58" s="1">
         <f>(-125.35-114.61) / 2</f>
         <v>-119.97999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N61" t="s">
+        <v>20</v>
+      </c>
+      <c r="O61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>0.99</v>
+      </c>
+      <c r="C62">
+        <v>0.6</v>
+      </c>
+      <c r="D62">
+        <v>0.1</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>10000</v>
+      </c>
+      <c r="G62">
+        <v>256</v>
+      </c>
+      <c r="H62">
+        <v>128</v>
+      </c>
+      <c r="I62">
+        <v>1000</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62">
+        <v>1E-3</v>
+      </c>
+      <c r="L62" s="1">
+        <v>190.9</v>
+      </c>
+      <c r="M62" s="1">
+        <v>-119.98</v>
+      </c>
+      <c r="N62">
+        <f>(-228.86-237.575)/2</f>
+        <v>-233.2175</v>
+      </c>
+      <c r="O62" s="1">
+        <f>SUM(L62:N62)</f>
+        <v>-162.29750000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>0.6</v>
+      </c>
+      <c r="D63">
+        <v>0.1</v>
+      </c>
+      <c r="E63">
+        <v>100</v>
+      </c>
+      <c r="F63">
+        <v>10000</v>
+      </c>
+      <c r="G63">
+        <v>256</v>
+      </c>
+      <c r="H63">
+        <v>128</v>
+      </c>
+      <c r="I63">
+        <v>1000</v>
+      </c>
+      <c r="J63">
+        <v>4</v>
+      </c>
+      <c r="K63">
+        <v>1E-3</v>
+      </c>
+      <c r="L63" s="1">
+        <v>195.2</v>
+      </c>
+      <c r="M63" s="1">
+        <v>-199.65</v>
+      </c>
+      <c r="P63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M64" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>